<commit_message>
#130 try fix test
</commit_message>
<xml_diff>
--- a/tests/Gauges/tLists1_cell_setting.xlsx
+++ b/tests/Gauges/tLists1_cell_setting.xlsx
@@ -1232,8 +1232,8 @@
   <x:sheetViews>
     <x:sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <x:pane xSplit="0" ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozenSplit"/>
-      <x:selection activeCell="K13" sqref="K13"/>
-      <x:selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+      <x:selection activeCell="G29" sqref="G29"/>
+      <x:selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="11.25"/>

</xml_diff>

<commit_message>
#130 test fixed. Сulture is set to invariant
</commit_message>
<xml_diff>
--- a/tests/Gauges/tLists1_cell_setting.xlsx
+++ b/tests/Gauges/tLists1_cell_setting.xlsx
@@ -90,7 +90,7 @@
             <x:rFont val="Arial"/>
             <x:family val="2"/>
           </x:rPr>
-          <x:t>31219,95</x:t>
+          <x:t>31219.95</x:t>
         </x:r>
       </x:text>
     </x:comment>
@@ -132,7 +132,7 @@
             <x:rFont val="Arial"/>
             <x:family val="2"/>
           </x:rPr>
-          <x:t>4317,75</x:t>
+          <x:t>4317.75</x:t>
         </x:r>
       </x:text>
     </x:comment>

</xml_diff>